<commit_message>
now compatible with python 3.7, 3.8, 3.9, 3.10
</commit_message>
<xml_diff>
--- a/source/py/notes/matrix.xlsx
+++ b/source/py/notes/matrix.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sa/Downloads/projects/py-js/source/py/notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A717CD2F-C734-BC4B-9092-CB6491812559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41902CC4-764C-EB40-BD15-1930B329D0AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1960" yWindow="1720" windowWidth="25000" windowHeight="13420" xr2:uid="{656454C3-FA4A-114C-8459-B2A646AF5476}"/>
+    <workbookView xWindow="860" yWindow="3800" windowWidth="15660" windowHeight="11380" xr2:uid="{656454C3-FA4A-114C-8459-B2A646AF5476}"/>
   </bookViews>
   <sheets>
-    <sheet name="matrix" sheetId="1" r:id="rId1"/>
-    <sheet name="targets" sheetId="2" r:id="rId2"/>
+    <sheet name="testing" sheetId="3" r:id="rId1"/>
+    <sheet name="matrix" sheetId="1" r:id="rId2"/>
+    <sheet name="targets" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="74">
   <si>
     <t>static</t>
   </si>
@@ -231,6 +232,33 @@
   </si>
   <si>
     <t>python3 -m builder pyjs_framework_pkg-i -b</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>pymx</t>
+  </si>
+  <si>
+    <t>python versions</t>
+  </si>
+  <si>
+    <t>3.9.10</t>
+  </si>
+  <si>
+    <t>3.10.3</t>
+  </si>
+  <si>
+    <t>3.7.8</t>
+  </si>
+  <si>
+    <t>3.8.10</t>
+  </si>
+  <si>
+    <t>pnf: patch not found</t>
   </si>
 </sst>
 </file>
@@ -240,7 +268,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -274,6 +302,14 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -380,7 +416,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -432,35 +468,74 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -769,13 +844,221 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71C7EDD8-2303-1D4E-BD35-415BCD4B1B09}">
+  <dimension ref="B2:F16"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="C2" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+    </row>
+    <row r="3" spans="2:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="B3" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="2:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5">
+        <v>1</v>
+      </c>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="2:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5">
+        <v>1</v>
+      </c>
+      <c r="F7" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1</v>
+      </c>
+      <c r="D8" s="5">
+        <v>1</v>
+      </c>
+      <c r="E8" s="5">
+        <v>1</v>
+      </c>
+      <c r="F8" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="5">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5">
+        <v>1</v>
+      </c>
+      <c r="E9" s="5">
+        <v>1</v>
+      </c>
+      <c r="F9" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="5">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5">
+        <v>1</v>
+      </c>
+      <c r="E10" s="5">
+        <v>1</v>
+      </c>
+      <c r="F10" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="5">
+        <v>1</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
+      <c r="E11" s="5">
+        <v>1</v>
+      </c>
+      <c r="F11" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5">
+        <v>1</v>
+      </c>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="2:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="5">
+        <v>1</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5">
+        <v>1</v>
+      </c>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="16" spans="2:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="B16" s="32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:F2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C4:F13">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{070FA639-8EF0-8844-B058-F13033E5A0B3}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:N21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -841,7 +1124,7 @@
       </c>
     </row>
     <row r="4" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="21" t="s">
         <v>56</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -850,10 +1133,10 @@
       <c r="D4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="24" t="s">
         <v>53</v>
       </c>
       <c r="G4" s="5" t="s">
@@ -882,15 +1165,15 @@
       </c>
     </row>
     <row r="5" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="B5" s="27"/>
+      <c r="B5" s="21"/>
       <c r="C5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
       <c r="G5" s="5" t="s">
         <v>3</v>
       </c>
@@ -917,7 +1200,7 @@
       </c>
     </row>
     <row r="6" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="21" t="s">
         <v>57</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -926,10 +1209,10 @@
       <c r="D6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E6" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="25" t="s">
+      <c r="F6" s="24" t="s">
         <v>54</v>
       </c>
       <c r="G6" s="5" t="s">
@@ -958,15 +1241,15 @@
       </c>
     </row>
     <row r="7" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="B7" s="27"/>
+      <c r="B7" s="21"/>
       <c r="C7" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
       <c r="G7" s="5" t="s">
         <v>3</v>
       </c>
@@ -993,7 +1276,7 @@
       </c>
     </row>
     <row r="8" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="21" t="s">
         <v>58</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1002,10 +1285,10 @@
       <c r="D8" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="25" t="s">
+      <c r="F8" s="24" t="s">
         <v>55</v>
       </c>
       <c r="G8" s="5" t="s">
@@ -1029,20 +1312,20 @@
       <c r="M8" s="5">
         <v>1</v>
       </c>
-      <c r="N8" s="28">
+      <c r="N8" s="22">
         <v>13.9</v>
       </c>
     </row>
     <row r="9" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="B9" s="27"/>
+      <c r="B9" s="21"/>
       <c r="C9" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
       <c r="G9" s="5" t="s">
         <v>3</v>
       </c>
@@ -1064,10 +1347,10 @@
       <c r="M9" s="5">
         <v>1</v>
       </c>
-      <c r="N9" s="28"/>
+      <c r="N9" s="22"/>
     </row>
     <row r="10" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="21" t="s">
         <v>59</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -1076,10 +1359,10 @@
       <c r="D10" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="F10" s="25" t="s">
+      <c r="F10" s="24" t="s">
         <v>25</v>
       </c>
       <c r="G10" s="5" t="s">
@@ -1108,15 +1391,15 @@
       </c>
     </row>
     <row r="11" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="B11" s="27"/>
+      <c r="B11" s="21"/>
       <c r="C11" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
       <c r="G11" s="5" t="s">
         <v>3</v>
       </c>
@@ -1143,7 +1426,7 @@
       </c>
     </row>
     <row r="12" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="21" t="s">
         <v>60</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -1152,10 +1435,10 @@
       <c r="D12" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="25" t="s">
+      <c r="E12" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="F12" s="25" t="s">
+      <c r="F12" s="24" t="s">
         <v>26</v>
       </c>
       <c r="G12" s="5" t="s">
@@ -1184,15 +1467,15 @@
       </c>
     </row>
     <row r="13" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="B13" s="27"/>
+      <c r="B13" s="21"/>
       <c r="C13" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
       <c r="G13" s="5" t="s">
         <v>3</v>
       </c>
@@ -1219,7 +1502,7 @@
       </c>
     </row>
     <row r="14" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="21" t="s">
         <v>61</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -1228,10 +1511,10 @@
       <c r="D14" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="25" t="s">
+      <c r="E14" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="F14" s="25" t="s">
+      <c r="F14" s="24" t="s">
         <v>27</v>
       </c>
       <c r="G14" s="5" t="s">
@@ -1260,15 +1543,15 @@
       </c>
     </row>
     <row r="15" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="B15" s="27"/>
+      <c r="B15" s="21"/>
       <c r="C15" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
       <c r="G15" s="5" t="s">
         <v>3</v>
       </c>
@@ -1295,7 +1578,7 @@
       </c>
     </row>
     <row r="16" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="21" t="s">
         <v>62</v>
       </c>
       <c r="C16" s="3" t="s">
@@ -1304,10 +1587,10 @@
       <c r="D16" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="25" t="s">
+      <c r="E16" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="F16" s="25" t="s">
+      <c r="F16" s="24" t="s">
         <v>28</v>
       </c>
       <c r="G16" s="5" t="s">
@@ -1331,21 +1614,21 @@
       <c r="M16" s="5">
         <v>1</v>
       </c>
-      <c r="N16" s="28">
+      <c r="N16" s="22">
         <f>18.7</f>
         <v>18.7</v>
       </c>
     </row>
     <row r="17" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="B17" s="27"/>
+      <c r="B17" s="21"/>
       <c r="C17" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
       <c r="G17" s="5" t="s">
         <v>3</v>
       </c>
@@ -1367,7 +1650,7 @@
       <c r="M17" s="5">
         <v>1</v>
       </c>
-      <c r="N17" s="28"/>
+      <c r="N17" s="22"/>
     </row>
     <row r="18" spans="2:14" ht="19" x14ac:dyDescent="0.25">
       <c r="B18" s="23" t="s">
@@ -1377,10 +1660,10 @@
         <v>18</v>
       </c>
       <c r="D18" s="13"/>
-      <c r="E18" s="21" t="s">
+      <c r="E18" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="F18" s="21" t="s">
+      <c r="F18" s="26" t="s">
         <v>29</v>
       </c>
       <c r="G18" s="9" t="s">
@@ -1410,8 +1693,8 @@
         <v>18</v>
       </c>
       <c r="D19" s="13"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
       <c r="G19" s="9" t="s">
         <v>3</v>
       </c>
@@ -1443,10 +1726,10 @@
       <c r="D20" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="21" t="s">
+      <c r="E20" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="F20" s="21" t="s">
+      <c r="F20" s="26" t="s">
         <v>30</v>
       </c>
       <c r="G20" s="9" t="s">
@@ -1470,7 +1753,7 @@
       <c r="M20" s="9">
         <v>1</v>
       </c>
-      <c r="N20" s="24"/>
+      <c r="N20" s="28"/>
     </row>
     <row r="21" spans="2:14" ht="19" x14ac:dyDescent="0.25">
       <c r="B21" s="23"/>
@@ -1480,8 +1763,8 @@
       <c r="D21" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
       <c r="G21" s="9" t="s">
         <v>3</v>
       </c>
@@ -1503,24 +1786,10 @@
       <c r="M21" s="9">
         <v>1</v>
       </c>
-      <c r="N21" s="24"/>
+      <c r="N21" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="F10:F11"/>
     <mergeCell ref="F20:F21"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="N20:N21"/>
@@ -1537,13 +1806,27 @@
     <mergeCell ref="E16:E17"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="F18:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="58" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11C27982-693A-F04A-877F-4F325C25078C}">
   <dimension ref="B2:E19"/>
   <sheetViews>

</xml_diff>